<commit_message>
starting on 2024 rolldown NCC update
</commit_message>
<xml_diff>
--- a/documentation/metadata/metadata-template.xlsx
+++ b/documentation/metadata/metadata-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobhoutman/Desktop/Git Hub/BC-river-level-SR/documentation/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobhoutman/Documents/Git Hub/BC-river-level-SR/documentation/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53200CB-6D2F-4347-94B6-3FF3F093E6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEEA9AE-5A36-454F-ADD9-0F9A867CDEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="500" windowWidth="37780" windowHeight="15980" xr2:uid="{360E2C9C-D489-0A43-994A-1536DFFABA6A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{360E2C9C-D489-0A43-994A-1536DFFABA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_info" sheetId="1" r:id="rId1"/>
@@ -948,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E3E850-C45F-A240-BE06-3818AE3F2997}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1107,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CC1A69-F024-FF4E-84CA-451DDD8B3A75}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>